<commit_message>
Updated Test Data For Finland Market
</commit_message>
<xml_diff>
--- a/Test Data/Gallery_Panels.xlsx
+++ b/Test Data/Gallery_Panels.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\consys-uiauto\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EB2BD63-85B0-4B5F-8A57-BABC61B9AF4E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1C7F3F8-5B99-4CA8-8080-7B4232CC9717}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="9" activeTab="19" xr2:uid="{C41C5F48-4FD1-41E2-932B-493D5E69981C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="9" activeTab="15" xr2:uid="{C41C5F48-4FD1-41E2-932B-493D5E69981C}"/>
   </bookViews>
   <sheets>
     <sheet name="Germany" sheetId="7" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="749" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="747" uniqueCount="87">
   <si>
     <t>Wg</t>
   </si>
@@ -2225,10 +2225,10 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A1271AC-FFEC-44CE-91CF-FA4FCCBE2833}">
-  <dimension ref="A1:D32"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection sqref="A1:D33"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2381,41 +2381,31 @@
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
-        <v>30</v>
+        <v>73</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
-        <v>39</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A31" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A32" s="3" t="s">
         <v>35</v>
       </c>
     </row>
@@ -3288,7 +3278,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03E168F3-F31A-4459-A4F6-B1E12285BF7D}">
   <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>

</xml_diff>